<commit_message>
Added the rest of the MS failure notes
</commit_message>
<xml_diff>
--- a/Failure_notes.xlsx
+++ b/Failure_notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="18195" windowHeight="13605"/>
+    <workbookView xWindow="6270" yWindow="-180" windowWidth="18195" windowHeight="13605"/>
   </bookViews>
   <sheets>
     <sheet name="Standard MS failure Notes" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="155">
   <si>
     <t>Failure</t>
   </si>
@@ -105,9 +105,6 @@
     <t>poor CFR610 coupling</t>
   </si>
   <si>
-    <t>r CFR610</t>
-  </si>
-  <si>
     <t>Quasar 570 coupling failure</t>
   </si>
   <si>
@@ -123,15 +120,419 @@
     <t>poor BHQ3 coupling</t>
   </si>
   <si>
-    <t>r BHQ3</t>
+    <t>poor Cal Fluor Orange 560 coupling</t>
+  </si>
+  <si>
+    <t>poor CFO560 coupling</t>
+  </si>
+  <si>
+    <t>r bhq3</t>
+  </si>
+  <si>
+    <t>r cfr610</t>
+  </si>
+  <si>
+    <t>r cfo</t>
+  </si>
+  <si>
+    <t>BHQ2 coupling failure</t>
+  </si>
+  <si>
+    <t>poor BHQ2 coupling</t>
+  </si>
+  <si>
+    <t>r bhq2</t>
+  </si>
+  <si>
+    <t>BHQ1 coupling failure</t>
+  </si>
+  <si>
+    <t>poor BHQ1 coupling</t>
+  </si>
+  <si>
+    <t>r bhq1</t>
+  </si>
+  <si>
+    <t>FAM coupling failure</t>
+  </si>
+  <si>
+    <t>poor FAM coupling</t>
+  </si>
+  <si>
+    <t>Cal Fluor Gold 540 coupling failure</t>
+  </si>
+  <si>
+    <t>poor CFG540 coupling</t>
+  </si>
+  <si>
+    <t>r cfg</t>
+  </si>
+  <si>
+    <t>r fam</t>
+  </si>
+  <si>
+    <t>ROX coupling failure</t>
+  </si>
+  <si>
+    <t>poor ROX coupling</t>
+  </si>
+  <si>
+    <t>r rox</t>
+  </si>
+  <si>
+    <t>Joe coupling failure</t>
+  </si>
+  <si>
+    <t>poor JOE coupling</t>
+  </si>
+  <si>
+    <t>poor joe</t>
+  </si>
+  <si>
+    <t>Biotin coupling failure</t>
+  </si>
+  <si>
+    <t>poor Biotin coupling</t>
+  </si>
+  <si>
+    <t>r biotin</t>
+  </si>
+  <si>
+    <t>spacer 18 coupling failure</t>
+  </si>
+  <si>
+    <t>poor sp18</t>
+  </si>
+  <si>
+    <t>r sp18</t>
+  </si>
+  <si>
+    <t>N-1 synthsis failure</t>
+  </si>
+  <si>
+    <t>N-1 failure</t>
+  </si>
+  <si>
+    <t>n-1 f</t>
+  </si>
+  <si>
+    <t>mixed n-1 failure</t>
+  </si>
+  <si>
+    <t>mixed n-1</t>
+  </si>
+  <si>
+    <t>d n-1</t>
+  </si>
+  <si>
+    <t>seqential n-1 failure</t>
+  </si>
+  <si>
+    <t>l n-1</t>
+  </si>
+  <si>
+    <t>sequential n-1</t>
+  </si>
+  <si>
+    <t>Depurination</t>
+  </si>
+  <si>
+    <t>depurination</t>
+  </si>
+  <si>
+    <t>depuri</t>
+  </si>
+  <si>
+    <t>phosphate coupling failure</t>
+  </si>
+  <si>
+    <t>poor phosphate coupling</t>
+  </si>
+  <si>
+    <t>r phosp</t>
+  </si>
+  <si>
+    <t>TET/HEX impurity</t>
+  </si>
+  <si>
+    <t>tet/hex</t>
+  </si>
+  <si>
+    <t>Tiolated longmers</t>
+  </si>
+  <si>
+    <t>fully phosphothioliated longmers</t>
+  </si>
+  <si>
+    <t>Sodium adducts</t>
+  </si>
+  <si>
+    <t>sodium adducts</t>
+  </si>
+  <si>
+    <t>sodium</t>
+  </si>
+  <si>
+    <t>Potassium adducts</t>
+  </si>
+  <si>
+    <t>potassium adducts</t>
+  </si>
+  <si>
+    <t>potassium</t>
+  </si>
+  <si>
+    <t>Acetyl incomplete deprotection</t>
+  </si>
+  <si>
+    <t>Cyanoethyl incomplete deprotection</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Triazine incomplete deprotection</t>
+  </si>
+  <si>
+    <t>Benzoyl incomplete deprotection</t>
+  </si>
+  <si>
+    <t>HFIP buffer adduct</t>
+  </si>
+  <si>
+    <t>HFIP adduct</t>
+  </si>
+  <si>
+    <t>HFIP a</t>
+  </si>
+  <si>
+    <t>MMT left on</t>
+  </si>
+  <si>
+    <t>mmt l</t>
+  </si>
+  <si>
+    <t>DMT left on</t>
+  </si>
+  <si>
+    <t>dmt l</t>
+  </si>
+  <si>
+    <t>Uridine left on</t>
+  </si>
+  <si>
+    <t>ine l</t>
+  </si>
+  <si>
+    <t>extra FAM coupled</t>
+  </si>
+  <si>
+    <t>extra FAM coupling</t>
+  </si>
+  <si>
+    <t>a FAM</t>
+  </si>
+  <si>
+    <t>extra TET</t>
+  </si>
+  <si>
+    <t>extra TET coupling</t>
+  </si>
+  <si>
+    <t>a TET</t>
+  </si>
+  <si>
+    <t>MS okay notes</t>
+  </si>
+  <si>
+    <t>ms ok, ms okay, ms o</t>
+  </si>
+  <si>
+    <t>ms o</t>
+  </si>
+  <si>
+    <t>ms not okay notes</t>
+  </si>
+  <si>
+    <t>ms not okay, ms not, ms n</t>
+  </si>
+  <si>
+    <t>ms n</t>
+  </si>
+  <si>
+    <t>Wobble okay notes</t>
+  </si>
+  <si>
+    <t>wobble okay, wobble o</t>
+  </si>
+  <si>
+    <t>wobble o</t>
+  </si>
+  <si>
+    <r>
+      <t>Wobble failures (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>do we want these catagorized?)</t>
+    </r>
+  </si>
+  <si>
+    <t>wobble failure</t>
+  </si>
+  <si>
+    <t>wobble f</t>
+  </si>
+  <si>
+    <t>Stellaris okay notes</t>
+  </si>
+  <si>
+    <t>stellaris okay</t>
+  </si>
+  <si>
+    <t>aris o</t>
+  </si>
+  <si>
+    <t>Stellaris failure notes</t>
+  </si>
+  <si>
+    <t>stellaris failure</t>
+  </si>
+  <si>
+    <t>aris f</t>
+  </si>
+  <si>
+    <t>Base swap notes</t>
+  </si>
+  <si>
+    <t>baseswap</t>
+  </si>
+  <si>
+    <t>basesw</t>
+  </si>
+  <si>
+    <t>No FLP, no product, etc</t>
+  </si>
+  <si>
+    <t>no FLP</t>
+  </si>
+  <si>
+    <t>o FLP</t>
+  </si>
+  <si>
+    <t>wrong mass (unspecified failure)</t>
+  </si>
+  <si>
+    <t>wrong mass</t>
+  </si>
+  <si>
+    <t>wrong m</t>
+  </si>
+  <si>
+    <t>Poor fluorescense</t>
+  </si>
+  <si>
+    <t>poor fluorescense</t>
+  </si>
+  <si>
+    <t>poor fl</t>
+  </si>
+  <si>
+    <t>N-2 synthesis failure</t>
+  </si>
+  <si>
+    <t>N-2 failure</t>
+  </si>
+  <si>
+    <t>n-2 f</t>
+  </si>
+  <si>
+    <t>N-3 synthesis failure</t>
+  </si>
+  <si>
+    <t>N-3 failure</t>
+  </si>
+  <si>
+    <t>n-3 f</t>
+  </si>
+  <si>
+    <t>Scrambled plate</t>
+  </si>
+  <si>
+    <t>plate scrambled</t>
+  </si>
+  <si>
+    <t>te scram</t>
+  </si>
+  <si>
+    <t>impurity at known mass</t>
+  </si>
+  <si>
+    <t>impurity at (#)</t>
+  </si>
+  <si>
+    <t>impurity at</t>
+  </si>
+  <si>
+    <t>r purity</t>
+  </si>
+  <si>
+    <r>
+      <t>poor purity (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>do we want to know if its our or their spec?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>General failure</t>
+  </si>
+  <si>
+    <t>synthesis failure</t>
+  </si>
+  <si>
+    <t>sis fai</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -462,15 +863,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" customWidth="1"/>
+    <col min="1" max="1" width="58.7109375" customWidth="1"/>
     <col min="2" max="2" width="34.28515625" customWidth="1"/>
     <col min="3" max="3" width="42.5703125" customWidth="1"/>
   </cols>
@@ -488,127 +889,597 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>112</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>120</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>124</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>126</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>127</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>132</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>133</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>136</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" t="s">
+        <v>150</v>
+      </c>
+      <c r="C13" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B14" t="s">
+        <v>148</v>
+      </c>
+      <c r="C14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B27" t="s">
         <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40" t="s">
+        <v>142</v>
+      </c>
+      <c r="C40" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>88</v>
+      </c>
+      <c r="B47" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>89</v>
+      </c>
+      <c r="B48" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>102</v>
+      </c>
+      <c r="B55" t="s">
+        <v>103</v>
+      </c>
+      <c r="C55" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" t="s">
+        <v>106</v>
+      </c>
+      <c r="C56" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added incomplete R replacement column, to perhaps in the future implement using this file to do name replacement.
</commit_message>
<xml_diff>
--- a/Failure_notes.xlsx
+++ b/Failure_notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6270" yWindow="-180" windowWidth="18195" windowHeight="13605"/>
+    <workbookView xWindow="1770" yWindow="-30" windowWidth="18195" windowHeight="13605"/>
   </bookViews>
   <sheets>
     <sheet name="Standard MS failure Notes" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="177">
   <si>
     <t>Failure</t>
   </si>
@@ -517,6 +517,72 @@
   </si>
   <si>
     <t>sis fai</t>
+  </si>
+  <si>
+    <t>R replacement</t>
+  </si>
+  <si>
+    <t>MS Okay note</t>
+  </si>
+  <si>
+    <t>MS note okay note</t>
+  </si>
+  <si>
+    <t>Wobble okay note</t>
+  </si>
+  <si>
+    <t>Wobble failure</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Stellaris Failures</t>
+  </si>
+  <si>
+    <t>Baseswap</t>
+  </si>
+  <si>
+    <t>No full length product</t>
+  </si>
+  <si>
+    <t>Wrong Mass found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poor Fluoresence </t>
+  </si>
+  <si>
+    <t>Plate scrambled</t>
+  </si>
+  <si>
+    <t>Poor Purity</t>
+  </si>
+  <si>
+    <t>Impurity at specific mass</t>
+  </si>
+  <si>
+    <t>General Synthesis Failure</t>
+  </si>
+  <si>
+    <t>Poor Texas Red coupling</t>
+  </si>
+  <si>
+    <t>Poor Pulsar Coupling</t>
+  </si>
+  <si>
+    <t>Poor Methlyene Blue Coupling</t>
+  </si>
+  <si>
+    <t>poor Quasar 705 Coupling</t>
+  </si>
+  <si>
+    <t>Poor HEX coupling</t>
+  </si>
+  <si>
+    <t>Poor TET coupling</t>
+  </si>
+  <si>
+    <t>Poor TAM coupling</t>
   </si>
 </sst>
 </file>
@@ -863,20 +929,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="58.7109375" customWidth="1"/>
     <col min="2" max="2" width="34.28515625" customWidth="1"/>
-    <col min="3" max="3" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="62.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -886,8 +953,11 @@
       <c r="C1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>108</v>
       </c>
@@ -897,8 +967,11 @@
       <c r="C2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>111</v>
       </c>
@@ -908,8 +981,11 @@
       <c r="C3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>114</v>
       </c>
@@ -919,8 +995,11 @@
       <c r="C4" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -930,8 +1009,11 @@
       <c r="C5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>120</v>
       </c>
@@ -941,8 +1023,11 @@
       <c r="C6" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>123</v>
       </c>
@@ -952,8 +1037,11 @@
       <c r="C7" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>126</v>
       </c>
@@ -963,8 +1051,11 @@
       <c r="C8" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>129</v>
       </c>
@@ -974,8 +1065,11 @@
       <c r="C9" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>132</v>
       </c>
@@ -985,8 +1079,11 @@
       <c r="C10" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>135</v>
       </c>
@@ -996,8 +1093,11 @@
       <c r="C11" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>144</v>
       </c>
@@ -1007,8 +1107,11 @@
       <c r="C12" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>151</v>
       </c>
@@ -1018,8 +1121,11 @@
       <c r="C13" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>147</v>
       </c>
@@ -1029,8 +1135,11 @@
       <c r="C14" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>152</v>
       </c>
@@ -1040,8 +1149,11 @@
       <c r="C15" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1051,8 +1163,11 @@
       <c r="C16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1062,8 +1177,11 @@
       <c r="C17" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1073,8 +1191,11 @@
       <c r="C18" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1084,8 +1205,11 @@
       <c r="C19" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -1095,8 +1219,11 @@
       <c r="C20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1106,8 +1233,11 @@
       <c r="C21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1117,8 +1247,11 @@
       <c r="C22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1129,7 +1262,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1140,7 +1273,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -1151,7 +1284,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1162,7 +1295,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1173,7 +1306,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>39</v>
       </c>
@@ -1184,7 +1317,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -1195,7 +1328,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -1206,7 +1339,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -1217,7 +1350,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>51</v>
       </c>

</xml_diff>